<commit_message>
Move files + comment: oanh, phúc, thảo, phương thảo
</commit_message>
<xml_diff>
--- a/DS SV.xlsx
+++ b/DS SV.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8820" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$17</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
   <si>
     <t>STT</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Buổi 2</t>
+  </si>
+  <si>
+    <t>Buổi 3</t>
   </si>
   <si>
     <t>Trần Văn Lực</t>
@@ -75,6 +78,9 @@
   </si>
   <si>
     <t>Cần confirm: sau khi học xong thì có được giao dự án để thực hành? Có môi trường giả lập để chỉnh sửa hay không?</t>
+  </si>
+  <si>
+    <t>Gần OK</t>
   </si>
   <si>
     <t>Đoàn Thị Thanh Tâm</t>
@@ -141,6 +147,9 @@
   <si>
     <t>Công ty không cho thông tin dự án thật.
 --&gt; Xin một web khác của công ty (có thể do nhóm thực tập khác làm ra) để test</t>
+  </si>
+  <si>
+    <t>Đã comment, cần làm lại.</t>
   </si>
   <si>
     <t>Võ Thị Phúc</t>
@@ -252,6 +261,9 @@
 --&gt; Làm đề tài triển khai kế toán cho công ty XYZ</t>
   </si>
   <si>
+    <t>Sẽ upload file vào tối</t>
+  </si>
+  <si>
     <t>Hồ Ngọc Hoàng Vũ</t>
   </si>
   <si>
@@ -316,6 +328,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+      </rPr>
       <t>42K21</t>
     </r>
     <r>
@@ -342,10 +359,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -398,14 +415,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,7 +451,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -441,11 +497,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -464,82 +557,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -574,187 +591,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,8 +840,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -840,6 +890,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -869,68 +934,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -940,134 +957,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1149,6 +1166,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1166,6 +1186,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1491,21 +1520,22 @@
   <sheetPr/>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.14285714285714" customWidth="1"/>
     <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="9.14285714285714" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="3" max="3" width="9.14285714285714" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="7" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="48.7142857142857" customWidth="1"/>
-    <col min="8" max="8" width="29.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="28.2857142857143" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="48.7142857142857" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="29.4285714285714" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="51.2857142857143" style="9" customWidth="1"/>
+    <col min="10" max="10" width="22.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1533,36 +1563,38 @@
       <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11"/>
+      <c r="J1" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="14">
         <v>2.94</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="36"/>
     </row>
@@ -1571,75 +1603,79 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="18">
         <v>2.74</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="I3" s="39"/>
+      <c r="J3" s="36" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="18">
         <v>2.56</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="36"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="36" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="18">
         <v>2.36</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
-      <c r="I5" s="39"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="36"/>
     </row>
     <row r="6" s="8" customFormat="1" spans="1:10">
@@ -1647,84 +1683,84 @@
         <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" s="26">
         <v>2.26</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="27"/>
       <c r="H6" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="41"/>
+        <v>14</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="42"/>
     </row>
     <row r="7" s="8" customFormat="1" ht="51" customHeight="1" spans="1:10">
       <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="26">
         <v>2.93</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="41"/>
+        <v>30</v>
+      </c>
+      <c r="I7" s="43"/>
+      <c r="J7" s="42"/>
     </row>
     <row r="8" ht="60" spans="1:10">
       <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="18">
         <v>2.16</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J8" s="36"/>
     </row>
@@ -1733,112 +1769,116 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="18">
         <v>2.71</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="36"/>
+        <v>39</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" ht="32" customHeight="1" spans="1:10">
       <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="18">
         <v>2.69</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H10" s="24"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="36"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" ht="30" spans="1:10">
       <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D11" s="18">
         <v>2.9</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="36"/>
+        <v>46</v>
+      </c>
+      <c r="J11" s="36" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" ht="45" spans="1:10">
       <c r="A12" s="12">
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D12" s="18">
         <v>2.81</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>51</v>
       </c>
       <c r="J12" s="36"/>
     </row>
@@ -1847,58 +1887,60 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" s="18">
         <v>2.48</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="36"/>
+        <v>57</v>
+      </c>
+      <c r="J13" s="36" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" ht="30" spans="1:10">
       <c r="A14" s="12">
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" s="18">
         <v>2.47</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J14" s="36"/>
     </row>
@@ -1907,70 +1949,84 @@
         <v>14</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="32">
         <v>1.98</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" s="36"/>
+        <v>68</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="12">
         <v>15</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C16" s="36"/>
       <c r="D16" s="36"/>
       <c r="E16" s="36" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
-      <c r="I16" s="43" t="s">
-        <v>68</v>
+      <c r="I16" s="46" t="s">
+        <v>72</v>
       </c>
       <c r="J16" s="36"/>
     </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
+    <row r="17" spans="1:10">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="37"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G16">
-    <sortState ref="A1:G16">
+  <autoFilter ref="A1:G17">
+    <sortState ref="A1:G17">
       <sortCondition ref="E2:E16"/>
     </sortState>
     <extLst/>
   </autoFilter>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="G3:G5"/>
     <mergeCell ref="H3:H5"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I2:I5"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1982,8 +2038,8 @@
   <sheetPr/>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1996,19 +2052,19 @@
         <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="5" t="str">
@@ -2025,19 +2081,19 @@
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5" t="str">
@@ -2054,16 +2110,16 @@
         <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
@@ -2081,16 +2137,16 @@
         <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
@@ -2108,19 +2164,19 @@
         <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="5" t="str">
@@ -2137,19 +2193,19 @@
         <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="5" t="str">
@@ -2166,19 +2222,19 @@
         <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="5" t="str">
@@ -2195,19 +2251,19 @@
         <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5" t="str">
@@ -2224,16 +2280,16 @@
         <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
@@ -2251,16 +2307,16 @@
         <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
@@ -2278,19 +2334,19 @@
         <v>74</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5" t="str">
@@ -2307,16 +2363,16 @@
         <v>75</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
@@ -2334,19 +2390,19 @@
         <v>76</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="5" t="str">
@@ -2363,16 +2419,16 @@
         <v>77</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
@@ -2390,16 +2446,16 @@
         <v>78</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
@@ -2417,20 +2473,20 @@
         <v>79</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H16" s="5" t="str">
         <f>VLOOKUP(B16,Sheet1!$B$2:$B$17,1,FALSE)</f>
@@ -2446,20 +2502,20 @@
         <v>80</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H17" s="5" t="e">
         <f>VLOOKUP(B17,Sheet1!$B$2:$B$17,1,FALSE)</f>

</xml_diff>

<commit_message>
Review đề cương sơ bộ
</commit_message>
<xml_diff>
--- a/DS SV.xlsx
+++ b/DS SV.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="102">
   <si>
     <t>STT</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Buổi 3</t>
+  </si>
+  <si>
+    <t>Check đề cương</t>
   </si>
   <si>
     <t>Trần Văn Lực</t>
@@ -70,6 +73,9 @@
 2. Muốn làm đề tài về C# thì công ty có giao không hay tự tìm?</t>
   </si>
   <si>
+    <t>Chưa có file</t>
+  </si>
+  <si>
     <t>Hoàng Thị Oanh</t>
   </si>
   <si>
@@ -81,6 +87,9 @@
   </si>
   <si>
     <t>Gần OK</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
   <si>
     <t>Đoàn Thị Thanh Tâm</t>
@@ -104,6 +113,10 @@
 </t>
   </si>
   <si>
+    <t>Đã gợi ý outline. 
+Cần format văn bản cho đúng quy định</t>
+  </si>
+  <si>
     <t>Nguyễn Thị Thảo Như</t>
   </si>
   <si>
@@ -150,6 +163,9 @@
   </si>
   <si>
     <t>Đã comment, cần làm lại.</t>
+  </si>
+  <si>
+    <t>Đã comment. Cần chỉnh sửa lại</t>
   </si>
   <si>
     <t>Võ Thị Phúc</t>
@@ -206,6 +222,9 @@
     <t>Cung cấp tên công cụ test</t>
   </si>
   <si>
+    <t>Chưa update</t>
+  </si>
+  <si>
     <t>Ngô Thị Kim Kha</t>
   </si>
   <si>
@@ -262,6 +281,9 @@
   </si>
   <si>
     <t>Sẽ upload file vào tối</t>
+  </si>
+  <si>
+    <t>Cơ bản OK. Có chỉnh lại 1 lỗi nhỏ trong outline</t>
   </si>
   <si>
     <t>Hồ Ngọc Hoàng Vũ</t>
@@ -359,10 +381,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -415,6 +437,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -430,35 +474,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -468,6 +483,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,6 +535,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -513,44 +573,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -591,13 +613,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,169 +709,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,26 +859,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -877,25 +899,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -918,8 +931,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -934,12 +947,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -957,134 +979,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1169,6 +1191,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1181,17 +1206,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1515,10 +1555,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J7"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1532,10 +1572,10 @@
     <col min="7" max="7" width="48.7142857142857" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="29.4285714285714" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="51.2857142857143" style="9" customWidth="1"/>
-    <col min="10" max="10" width="22.8571428571429" customWidth="1"/>
+    <col min="10" max="11" width="22.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1566,439 +1606,483 @@
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="14">
         <v>2.94</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="36"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="18">
         <v>2.74</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="38"/>
+        <v>20</v>
+      </c>
+      <c r="I3" s="39"/>
       <c r="J3" s="36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>21</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="18">
         <v>2.56</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
       <c r="J4" s="36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>21</v>
+      </c>
+      <c r="K4" s="36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="18">
         <v>2.36</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
-      <c r="I5" s="39"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="36"/>
-    </row>
-    <row r="6" s="8" customFormat="1" spans="1:10">
+      <c r="K5" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" s="8" customFormat="1" spans="1:11">
       <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="26">
         <v>2.26</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="27"/>
       <c r="H6" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="41"/>
-    </row>
-    <row r="7" s="8" customFormat="1" ht="51" customHeight="1" spans="1:10">
+        <v>15</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="42"/>
+      <c r="K6" s="43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="1" ht="51" customHeight="1" spans="1:11">
       <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>23</v>
       </c>
       <c r="D7" s="26">
         <v>2.93</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-    </row>
-    <row r="8" ht="60" spans="1:10">
+        <v>34</v>
+      </c>
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46"/>
+    </row>
+    <row r="8" ht="60" spans="1:11">
       <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="18">
         <v>2.16</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J8" s="36"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" s="18">
         <v>2.71</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" ht="32" customHeight="1" spans="1:10">
+        <v>43</v>
+      </c>
+      <c r="J9" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" ht="32" customHeight="1" spans="1:11">
       <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="18">
         <v>2.69</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H10" s="24"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="45"/>
-    </row>
-    <row r="11" ht="30" spans="1:10">
+      <c r="I10" s="40"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+    </row>
+    <row r="11" ht="30" spans="1:11">
       <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="18">
         <v>2.9</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="34" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" ht="45" spans="1:10">
+        <v>44</v>
+      </c>
+      <c r="K11" s="51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" ht="45" spans="1:11">
       <c r="A12" s="12">
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="18">
         <v>2.81</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="46" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="I12" s="52" t="s">
+        <v>56</v>
       </c>
       <c r="J12" s="36"/>
-    </row>
-    <row r="13" ht="60" spans="1:10">
+      <c r="K12" s="38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" ht="60" spans="1:11">
       <c r="A13" s="12">
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" s="18">
         <v>2.48</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" ht="30" spans="1:10">
+        <v>44</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="1:11">
       <c r="A14" s="12">
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="18">
         <v>2.47</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J14" s="36"/>
-    </row>
-    <row r="15" ht="30" spans="1:10">
+      <c r="K14" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="1:11">
       <c r="A15" s="12">
         <v>14</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="32">
         <v>1.98</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>75</v>
+      </c>
+      <c r="K15" s="51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" ht="45" spans="1:11">
       <c r="A16" s="12">
         <v>15</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C16" s="36"/>
       <c r="D16" s="36"/>
       <c r="E16" s="36" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
-      <c r="I16" s="46" t="s">
-        <v>72</v>
+      <c r="I16" s="52" t="s">
+        <v>79</v>
       </c>
       <c r="J16" s="36"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="12">
         <v>16</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -2006,8 +2090,11 @@
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
-      <c r="I17" s="46"/>
+      <c r="I17" s="52"/>
       <c r="J17" s="36"/>
+      <c r="K17" s="38" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G17">
@@ -2016,7 +2103,7 @@
     </sortState>
     <extLst/>
   </autoFilter>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="G3:G5"/>
     <mergeCell ref="H3:H5"/>
     <mergeCell ref="H9:H10"/>
@@ -2025,6 +2112,8 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2050,19 +2139,19 @@
         <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="5" t="str">
@@ -2079,19 +2168,19 @@
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5" t="str">
@@ -2108,16 +2197,16 @@
         <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
@@ -2135,16 +2224,16 @@
         <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
@@ -2162,19 +2251,19 @@
         <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="5" t="str">
@@ -2191,19 +2280,19 @@
         <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="5" t="str">
@@ -2220,19 +2309,19 @@
         <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="5" t="str">
@@ -2249,19 +2338,19 @@
         <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5" t="str">
@@ -2278,16 +2367,16 @@
         <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
@@ -2305,16 +2394,16 @@
         <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
@@ -2332,19 +2421,19 @@
         <v>74</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5" t="str">
@@ -2361,16 +2450,16 @@
         <v>75</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
@@ -2388,19 +2477,19 @@
         <v>76</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="5" t="str">
@@ -2417,16 +2506,16 @@
         <v>77</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
@@ -2444,16 +2533,16 @@
         <v>78</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
@@ -2471,20 +2560,20 @@
         <v>79</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="H16" s="5" t="str">
         <f>VLOOKUP(B16,Sheet1!$B$2:$B$17,1,FALSE)</f>
@@ -2500,20 +2589,20 @@
         <v>80</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="H17" s="5" t="e">
         <f>VLOOKUP(B17,Sheet1!$B$2:$B$17,1,FALSE)</f>

</xml_diff>

<commit_message>
Update tài liệu cho Hằng, Thị Thảo và Tâm
</commit_message>
<xml_diff>
--- a/DS SV.xlsx
+++ b/DS SV.xlsx
@@ -240,7 +240,7 @@
     <t>Cần lấy tên công ty và nghiệp vụ cần triển khai?</t>
   </si>
   <si>
-    <t>Phân hệ kế toán cho công ty Tuấn Huy.
+    <t>Quản lý tour và bán tour cho công ty Tuấn Huy.
 --&gt; đi theo hướng triển khai ERP thông thường
 Cần lưu lại minh chứng khi đi thu thập yêu cầu --&gt; tăng value cho báo cáo</t>
   </si>
@@ -381,10 +381,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -444,7 +444,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -452,14 +452,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -473,39 +466,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -536,22 +506,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -574,7 +552,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -613,31 +613,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,151 +787,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,30 +859,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -898,17 +874,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -937,13 +907,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -956,20 +945,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -979,134 +979,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1211,9 +1211,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1557,8 +1554,8 @@
   <sheetPr/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1788,7 +1785,7 @@
       </c>
       <c r="I7" s="44"/>
       <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
+      <c r="K7" s="45"/>
     </row>
     <row r="8" ht="60" spans="1:11">
       <c r="A8" s="12">
@@ -1851,10 +1848,10 @@
       <c r="I9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="48" t="s">
+      <c r="K9" s="47" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1882,8 +1879,8 @@
       </c>
       <c r="H10" s="24"/>
       <c r="I10" s="40"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="50"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="49"/>
     </row>
     <row r="11" ht="30" spans="1:11">
       <c r="A11" s="12">
@@ -1914,7 +1911,7 @@
       <c r="J11" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="51" t="s">
+      <c r="K11" s="50" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1943,7 +1940,7 @@
       <c r="H12" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="51" t="s">
         <v>56</v>
       </c>
       <c r="J12" s="36"/>
@@ -2050,7 +2047,7 @@
       <c r="J15" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="50" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2069,11 +2066,11 @@
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="51" t="s">
         <v>79</v>
       </c>
       <c r="J16" s="36"/>
-      <c r="K16" s="51" t="s">
+      <c r="K16" s="50" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2090,7 +2087,7 @@
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
-      <c r="I17" s="52"/>
+      <c r="I17" s="51"/>
       <c r="J17" s="36"/>
       <c r="K17" s="38" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Update đề cương sơ bộ + copy tài liệu tham khảo cho Thùy
</commit_message>
<xml_diff>
--- a/DS SV.xlsx
+++ b/DS SV.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="101">
   <si>
     <t>STT</t>
   </si>
@@ -73,7 +73,7 @@
 2. Muốn làm đề tài về C# thì công ty có giao không hay tự tìm?</t>
   </si>
   <si>
-    <t>Chưa có file</t>
+    <t>OK</t>
   </si>
   <si>
     <t>Hoàng Thị Oanh</t>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Gần OK</t>
-  </si>
-  <si>
-    <t>OK</t>
   </si>
   <si>
     <t>Đoàn Thị Thanh Tâm</t>
@@ -144,6 +141,9 @@
   <si>
     <t>Được phép tham gia dự án thật.
 Hỏi: triển khai phân hệ nào, của công ty nào?</t>
+  </si>
+  <si>
+    <t>Chưa có file</t>
   </si>
   <si>
     <t>Dương Phương Thảo</t>
@@ -283,16 +283,13 @@
     <t>Sẽ upload file vào tối</t>
   </si>
   <si>
-    <t>Cơ bản OK. Có chỉnh lại 1 lỗi nhỏ trong outline</t>
-  </si>
-  <si>
     <t>Hồ Ngọc Hoàng Vũ</t>
   </si>
   <si>
     <t>Efox</t>
   </si>
   <si>
-    <t>Xây dựng hệ thống quản lý nhân sự cho công ty nhỏ Efox</t>
+    <t>Xây dựng hệ thống quản lý mua sắm cho công ty Efox solution</t>
   </si>
   <si>
     <t>Lê Thị Mộng Thùy</t>
@@ -381,10 +378,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -437,7 +434,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,14 +457,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -467,7 +471,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -475,9 +479,46 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -505,31 +546,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -550,37 +576,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,12 +592,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -613,13 +604,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,121 +760,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,43 +784,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,6 +850,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -876,24 +891,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -901,8 +903,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -922,37 +924,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -961,15 +952,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -979,134 +970,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1121,22 +1112,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1162,17 +1153,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1188,10 +1176,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1200,19 +1188,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1554,8 +1542,8 @@
   <sheetPr/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1597,7 +1585,7 @@
       <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="34" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="11" t="s">
@@ -1633,8 +1621,8 @@
       <c r="I2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="38" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1663,12 +1651,12 @@
       <c r="H3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="36" t="s">
+      <c r="I3" s="36"/>
+      <c r="J3" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="36" t="s">
-        <v>22</v>
+      <c r="K3" s="33" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1676,7 +1664,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>12</v>
@@ -1692,12 +1680,12 @@
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="36" t="s">
+      <c r="I4" s="36"/>
+      <c r="J4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="36" t="s">
-        <v>22</v>
+      <c r="K4" s="33" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1705,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>12</v>
@@ -1721,78 +1709,78 @@
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="38" t="s">
+      <c r="I5" s="37"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" s="8" customFormat="1" spans="1:11">
-      <c r="A6" s="12">
+      <c r="A6" s="25">
         <v>5</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="D6" s="18">
+        <v>2.26</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="26">
-        <v>2.26</v>
-      </c>
-      <c r="E6" s="26" t="s">
+      <c r="F6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="41" t="s">
+      <c r="J6" s="39"/>
+      <c r="K6" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="42"/>
-      <c r="K6" s="43" t="s">
+    </row>
+    <row r="7" s="8" customFormat="1" ht="51" customHeight="1" spans="1:11">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" s="8" customFormat="1" ht="51" customHeight="1" spans="1:11">
-      <c r="A7" s="12">
-        <v>6</v>
-      </c>
-      <c r="B7" s="25" t="s">
+      <c r="C7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2.93</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="26">
-        <v>2.93</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="F7" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="G7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="H7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
     </row>
     <row r="8" ht="60" spans="1:11">
       <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>12</v>
@@ -1801,23 +1789,23 @@
         <v>2.16</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="I8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="J8" s="33"/>
+      <c r="K8" s="35" t="s">
         <v>38</v>
-      </c>
-      <c r="J8" s="36"/>
-      <c r="K8" s="38" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1828,7 +1816,7 @@
         <v>39</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="18">
         <v>2.71</v>
@@ -1836,10 +1824,10 @@
       <c r="E9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="30" t="s">
+      <c r="F9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="26" t="s">
         <v>41</v>
       </c>
       <c r="H9" s="20" t="s">
@@ -1848,10 +1836,10 @@
       <c r="I9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="J9" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="44" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1863,7 +1851,7 @@
         <v>46</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="18">
         <v>2.69</v>
@@ -1871,16 +1859,16 @@
       <c r="E10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="30" t="s">
+      <c r="F10" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="26" t="s">
         <v>47</v>
       </c>
       <c r="H10" s="24"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
     </row>
     <row r="11" ht="30" spans="1:11">
       <c r="A11" s="12">
@@ -1890,7 +1878,7 @@
         <v>48</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="18">
         <v>2.9</v>
@@ -1901,17 +1889,17 @@
       <c r="F11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="26" t="s">
         <v>50</v>
       </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="50" t="s">
+      <c r="K11" s="47" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1923,7 +1911,7 @@
         <v>52</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="18">
         <v>2.81</v>
@@ -1931,20 +1919,20 @@
       <c r="E12" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="30" t="s">
+      <c r="F12" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>54</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="51" t="s">
+      <c r="I12" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="36"/>
-      <c r="K12" s="38" t="s">
+      <c r="J12" s="33"/>
+      <c r="K12" s="35" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1956,7 +1944,7 @@
         <v>58</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="18">
         <v>2.48</v>
@@ -1967,7 +1955,7 @@
       <c r="F13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="26" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="16" t="s">
@@ -1976,11 +1964,11 @@
       <c r="I13" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="K13" s="36" t="s">
-        <v>22</v>
+      <c r="K13" s="33" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" ht="30" spans="1:11">
@@ -1991,7 +1979,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="18">
         <v>2.47</v>
@@ -2002,7 +1990,7 @@
       <c r="F14" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="26" t="s">
         <v>66</v>
       </c>
       <c r="H14" s="16" t="s">
@@ -2011,8 +1999,8 @@
       <c r="I14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="38" t="s">
+      <c r="J14" s="33"/>
+      <c r="K14" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2020,77 +2008,77 @@
       <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="29">
         <v>1.98</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="31" t="s">
         <v>73</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="K15" s="50" t="s">
-        <v>76</v>
+      <c r="K15" s="47" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" ht="45" spans="1:11">
       <c r="A16" s="12">
         <v>15</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36" t="s">
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16" s="36"/>
-      <c r="K16" s="50" t="s">
-        <v>29</v>
+      <c r="J16" s="33"/>
+      <c r="K16" s="47" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="38" t="s">
-        <v>17</v>
+      <c r="B17" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="35" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2142,10 +2130,10 @@
         <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>13</v>
@@ -2165,19 +2153,19 @@
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5" t="str">
@@ -2197,13 +2185,13 @@
         <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
@@ -2224,13 +2212,13 @@
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
@@ -2254,10 +2242,10 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
@@ -2280,13 +2268,13 @@
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>40</v>
@@ -2309,13 +2297,13 @@
         <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>40</v>
@@ -2335,16 +2323,16 @@
         <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
@@ -2367,13 +2355,13 @@
         <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
@@ -2394,13 +2382,13 @@
         <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
@@ -2418,16 +2406,16 @@
         <v>74</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>13</v>
@@ -2447,16 +2435,16 @@
         <v>75</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
@@ -2474,16 +2462,16 @@
         <v>76</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>13</v>
@@ -2503,16 +2491,16 @@
         <v>77</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
@@ -2536,10 +2524,10 @@
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
@@ -2557,20 +2545,20 @@
         <v>79</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H16" s="5" t="str">
         <f>VLOOKUP(B16,Sheet1!$B$2:$B$17,1,FALSE)</f>
@@ -2586,20 +2574,20 @@
         <v>80</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17" s="5" t="e">
         <f>VLOOKUP(B17,Sheet1!$B$2:$B$17,1,FALSE)</f>

</xml_diff>